<commit_message>
Version 1.02.            - Changed 'Talk' label to 'Direct instruction' in all the code.            - Created separate folders for png and tif figures.            - Changed project name to 'plos_one_2026.proj
</commit_message>
<xml_diff>
--- a/Tables/TableS3-Pairwise_between_LMM_Score.xlsx
+++ b/Tables/TableS3-Pairwise_between_LMM_Score.xlsx
@@ -587,7 +587,7 @@
         <is>
           <r>
             <rPr/>
-            <t>Abb. Workshop - Talk</t>
+            <t>Abb. Workshop - Direct instruction</t>
           </r>
         </is>
       </c>
@@ -661,7 +661,7 @@
         <is>
           <r>
             <rPr/>
-            <t>Workshop - Talk</t>
+            <t>Workshop - Direct Instruction</t>
           </r>
         </is>
       </c>
@@ -809,7 +809,7 @@
         <is>
           <r>
             <rPr/>
-            <t>Abb. Workshop - Talk</t>
+            <t>Abb. Workshop - Direct instruction</t>
           </r>
         </is>
       </c>
@@ -883,7 +883,7 @@
         <is>
           <r>
             <rPr/>
-            <t>Workshop - Talk</t>
+            <t>Workshop - Direct Instruction</t>
           </r>
         </is>
       </c>

</xml_diff>